<commit_message>
Adicionando as últimas atualizações no Cronograma e Wireframes.
</commit_message>
<xml_diff>
--- a/Cronograma de Desenvolvimento.xlsx
+++ b/Cronograma de Desenvolvimento.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno2\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno2\Desktop\tap\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,19 +24,73 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>CRONOGRAMA DE DESENVOLVIMENTO TAP</t>
   </si>
   <si>
     <t>Entrega atividades anteriores, formatação de Manual Técnico e Preparação Pitch Presentation</t>
+  </si>
+  <si>
+    <t>A fazer</t>
+  </si>
+  <si>
+    <t>Pesquisa de Projeto</t>
+  </si>
+  <si>
+    <t>Elaboração de Problematização</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Idealização de Projeto</t>
+  </si>
+  <si>
+    <t>Levantamento de Requisitos</t>
+  </si>
+  <si>
+    <t>Canvas</t>
+  </si>
+  <si>
+    <t>Mapa de Empatia</t>
+  </si>
+  <si>
+    <t>Fluxo de Usabilidade</t>
+  </si>
+  <si>
+    <t>Protipação de Telas</t>
+  </si>
+  <si>
+    <t>Elaboração da Identidade Visual</t>
+  </si>
+  <si>
+    <t>Diagrama de Caso de Uso</t>
+  </si>
+  <si>
+    <t>Diagrama de Classes</t>
+  </si>
+  <si>
+    <t>Diagrama Sequencial</t>
+  </si>
+  <si>
+    <t>Estruturação do Manual Técnico</t>
+  </si>
+  <si>
+    <t>Desenvolvimento de Banco de Dados</t>
+  </si>
+  <si>
+    <t>Desenvolvimento da Regra de Negócio</t>
+  </si>
+  <si>
+    <t>Desenvolvimento de MVP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,8 +110,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -73,6 +132,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -141,12 +224,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -154,17 +234,38 @@
     <xf numFmtId="16" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,7 +546,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:N53"/>
+  <dimension ref="C2:X53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D6" sqref="D6:N6"/>
@@ -456,332 +557,597 @@
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C2" s="2" t="s">
+    <row r="2" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="C2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-    </row>
-    <row r="3" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-    </row>
-    <row r="5" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C5" s="5">
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="P2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+    </row>
+    <row r="3" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+    </row>
+    <row r="4" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="P4" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11"/>
+    </row>
+    <row r="5" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="C5" s="4">
         <v>43768</v>
       </c>
-    </row>
-    <row r="6" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C6" s="5">
+      <c r="P5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="10"/>
+    </row>
+    <row r="6" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="C6" s="4">
         <v>43769</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="8"/>
-    </row>
-    <row r="8" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C8" s="4">
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="16"/>
+      <c r="P6" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="12"/>
+      <c r="V6" s="12"/>
+      <c r="W6" s="12"/>
+      <c r="X6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="P7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+    </row>
+    <row r="8" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="C8" s="3">
         <v>43770</v>
       </c>
-      <c r="D8" s="10"/>
-    </row>
-    <row r="9" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C9" s="4">
+      <c r="D8" s="6"/>
+      <c r="P8" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
+      <c r="W8" s="10"/>
+    </row>
+    <row r="9" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="C9" s="3">
         <v>43771</v>
       </c>
-      <c r="D9" s="10"/>
-    </row>
-    <row r="10" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C10" s="4">
+      <c r="D9" s="6"/>
+      <c r="P9" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
+      <c r="W9" s="10"/>
+    </row>
+    <row r="10" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="C10" s="3">
         <v>43772</v>
       </c>
-      <c r="D10" s="10"/>
-    </row>
-    <row r="11" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C11" s="4">
+      <c r="D10" s="6"/>
+      <c r="P10" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+    </row>
+    <row r="11" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="C11" s="3">
         <v>43773</v>
       </c>
-      <c r="D11" s="10"/>
-    </row>
-    <row r="12" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C12" s="4">
+      <c r="D11" s="6"/>
+      <c r="P11" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="11"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="11"/>
+    </row>
+    <row r="12" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="C12" s="3">
         <v>43774</v>
       </c>
-      <c r="D12" s="10"/>
-    </row>
-    <row r="13" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C13" s="4">
+      <c r="D12" s="6"/>
+      <c r="P12" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="11"/>
+      <c r="V12" s="11"/>
+      <c r="W12" s="11"/>
+    </row>
+    <row r="13" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="C13" s="3">
         <v>43775</v>
       </c>
-      <c r="D13" s="10"/>
-    </row>
-    <row r="14" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C14" s="4">
+      <c r="D13" s="6"/>
+      <c r="P13" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="13"/>
+      <c r="S13" s="13"/>
+      <c r="T13" s="13"/>
+      <c r="U13" s="13"/>
+      <c r="V13" s="13"/>
+      <c r="W13" s="13"/>
+    </row>
+    <row r="14" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="C14" s="3">
         <v>43776</v>
       </c>
-      <c r="D14" s="9"/>
-    </row>
-    <row r="15" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C15" s="4">
+      <c r="D14" s="5"/>
+      <c r="P14" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="13"/>
+      <c r="T14" s="13"/>
+      <c r="U14" s="13"/>
+      <c r="V14" s="13"/>
+      <c r="W14" s="13"/>
+    </row>
+    <row r="15" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="C15" s="3">
         <v>43777</v>
       </c>
-      <c r="D15" s="10"/>
-    </row>
-    <row r="16" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C16" s="4">
+      <c r="D15" s="6"/>
+      <c r="P15" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="13"/>
+      <c r="S15" s="13"/>
+      <c r="T15" s="13"/>
+      <c r="U15" s="13"/>
+      <c r="V15" s="13"/>
+      <c r="W15" s="13"/>
+    </row>
+    <row r="16" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="C16" s="3">
         <v>43778</v>
       </c>
-      <c r="D16" s="10"/>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C17" s="4">
+      <c r="D16" s="6"/>
+      <c r="P16" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="13"/>
+      <c r="S16" s="13"/>
+      <c r="T16" s="13"/>
+      <c r="U16" s="13"/>
+      <c r="V16" s="13"/>
+      <c r="W16" s="13"/>
+    </row>
+    <row r="17" spans="3:23" x14ac:dyDescent="0.2">
+      <c r="C17" s="3">
         <v>43779</v>
       </c>
-      <c r="D17" s="10"/>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C18" s="4">
+      <c r="D17" s="6"/>
+      <c r="P17" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="13"/>
+      <c r="S17" s="13"/>
+      <c r="T17" s="13"/>
+      <c r="U17" s="13"/>
+      <c r="V17" s="13"/>
+      <c r="W17" s="13"/>
+    </row>
+    <row r="18" spans="3:23" x14ac:dyDescent="0.2">
+      <c r="C18" s="3">
         <v>43780</v>
       </c>
-      <c r="D18" s="10"/>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C19" s="4">
+      <c r="D18" s="6"/>
+      <c r="P18" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q18" s="13"/>
+      <c r="R18" s="13"/>
+      <c r="S18" s="13"/>
+      <c r="T18" s="13"/>
+      <c r="U18" s="13"/>
+      <c r="V18" s="13"/>
+      <c r="W18" s="13"/>
+    </row>
+    <row r="19" spans="3:23" x14ac:dyDescent="0.2">
+      <c r="C19" s="3">
         <v>43781</v>
       </c>
-      <c r="D19" s="10"/>
-    </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C20" s="4">
+      <c r="D19" s="6"/>
+      <c r="P19" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="13"/>
+      <c r="S19" s="13"/>
+      <c r="T19" s="13"/>
+      <c r="U19" s="13"/>
+      <c r="V19" s="13"/>
+      <c r="W19" s="13"/>
+    </row>
+    <row r="20" spans="3:23" x14ac:dyDescent="0.2">
+      <c r="C20" s="3">
         <v>43782</v>
       </c>
-      <c r="D20" s="10"/>
-    </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C21" s="4">
+      <c r="D20" s="6"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="9"/>
+    </row>
+    <row r="21" spans="3:23" x14ac:dyDescent="0.2">
+      <c r="C21" s="3">
         <v>43783</v>
       </c>
-      <c r="D21" s="9"/>
-    </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C22" s="4">
+      <c r="D21" s="5"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
+      <c r="V21" s="9"/>
+      <c r="W21" s="9"/>
+    </row>
+    <row r="22" spans="3:23" x14ac:dyDescent="0.2">
+      <c r="C22" s="3">
         <v>43784</v>
       </c>
-      <c r="D22" s="10"/>
-    </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C23" s="4">
+      <c r="D22" s="6"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9"/>
+      <c r="W22" s="9"/>
+    </row>
+    <row r="23" spans="3:23" x14ac:dyDescent="0.2">
+      <c r="C23" s="3">
         <v>43785</v>
       </c>
-      <c r="D23" s="10"/>
-    </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C24" s="4">
+      <c r="D23" s="6"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9"/>
+      <c r="W23" s="9"/>
+    </row>
+    <row r="24" spans="3:23" x14ac:dyDescent="0.2">
+      <c r="C24" s="3">
         <v>43786</v>
       </c>
-      <c r="D24" s="10"/>
-    </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C25" s="4">
+      <c r="D24" s="6"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
+      <c r="U24" s="9"/>
+      <c r="V24" s="9"/>
+      <c r="W24" s="9"/>
+    </row>
+    <row r="25" spans="3:23" x14ac:dyDescent="0.2">
+      <c r="C25" s="3">
         <v>43787</v>
       </c>
-      <c r="D25" s="10"/>
-    </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C26" s="4">
+      <c r="D25" s="6"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="9"/>
+      <c r="V25" s="9"/>
+      <c r="W25" s="9"/>
+    </row>
+    <row r="26" spans="3:23" x14ac:dyDescent="0.2">
+      <c r="C26" s="3">
         <v>43788</v>
       </c>
-      <c r="D26" s="10"/>
-    </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C27" s="4">
+      <c r="D26" s="6"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
+      <c r="S26" s="9"/>
+      <c r="T26" s="9"/>
+      <c r="U26" s="9"/>
+      <c r="V26" s="9"/>
+      <c r="W26" s="9"/>
+    </row>
+    <row r="27" spans="3:23" x14ac:dyDescent="0.2">
+      <c r="C27" s="3">
         <v>43789</v>
       </c>
-      <c r="D27" s="10"/>
-    </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C28" s="4">
+      <c r="D27" s="6"/>
+    </row>
+    <row r="28" spans="3:23" x14ac:dyDescent="0.2">
+      <c r="C28" s="3">
         <v>43790</v>
       </c>
-      <c r="D28" s="9"/>
-    </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C29" s="4">
+      <c r="D28" s="5"/>
+    </row>
+    <row r="29" spans="3:23" x14ac:dyDescent="0.2">
+      <c r="C29" s="3">
         <v>43791</v>
       </c>
-      <c r="D29" s="10"/>
-    </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C30" s="4">
+      <c r="D29" s="6"/>
+    </row>
+    <row r="30" spans="3:23" x14ac:dyDescent="0.2">
+      <c r="C30" s="3">
         <v>43792</v>
       </c>
-      <c r="D30" s="10"/>
-    </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C31" s="4">
+      <c r="D30" s="6"/>
+    </row>
+    <row r="31" spans="3:23" x14ac:dyDescent="0.2">
+      <c r="C31" s="3">
         <v>43793</v>
       </c>
-      <c r="D31" s="10"/>
-    </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C32" s="4">
+      <c r="D31" s="6"/>
+    </row>
+    <row r="32" spans="3:23" x14ac:dyDescent="0.2">
+      <c r="C32" s="3">
         <v>43794</v>
       </c>
-      <c r="D32" s="10"/>
+      <c r="D32" s="6"/>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C33" s="4">
+      <c r="C33" s="3">
         <v>43795</v>
       </c>
-      <c r="D33" s="10"/>
+      <c r="D33" s="6"/>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C34" s="4">
+      <c r="C34" s="3">
         <v>43796</v>
       </c>
-      <c r="D34" s="10"/>
+      <c r="D34" s="6"/>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C35" s="4">
+      <c r="C35" s="3">
         <v>43797</v>
       </c>
-      <c r="D35" s="9"/>
+      <c r="D35" s="5"/>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C36" s="4">
+      <c r="C36" s="3">
         <v>43798</v>
       </c>
-      <c r="D36" s="10"/>
+      <c r="D36" s="6"/>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C37" s="4">
+      <c r="C37" s="3">
         <v>43799</v>
       </c>
-      <c r="D37" s="10"/>
+      <c r="D37" s="6"/>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C38" s="3"/>
+      <c r="C38" s="2"/>
     </row>
     <row r="39" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C39" s="5">
+      <c r="C39" s="4">
         <v>43800</v>
       </c>
-      <c r="D39" s="10"/>
+      <c r="D39" s="6"/>
     </row>
     <row r="40" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C40" s="5">
+      <c r="C40" s="4">
         <v>43801</v>
       </c>
-      <c r="D40" s="10"/>
+      <c r="D40" s="6"/>
     </row>
     <row r="41" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C41" s="5">
+      <c r="C41" s="4">
         <v>43802</v>
       </c>
-      <c r="D41" s="10"/>
+      <c r="D41" s="6"/>
     </row>
     <row r="42" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C42" s="5">
+      <c r="C42" s="4">
         <v>43803</v>
       </c>
-      <c r="D42" s="10"/>
+      <c r="D42" s="6"/>
     </row>
     <row r="43" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C43" s="5">
+      <c r="C43" s="4">
         <v>43804</v>
       </c>
-      <c r="D43" s="9"/>
+      <c r="D43" s="5"/>
     </row>
     <row r="44" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C44" s="5">
+      <c r="C44" s="4">
         <v>43805</v>
       </c>
-      <c r="D44" s="10"/>
+      <c r="D44" s="6"/>
     </row>
     <row r="45" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C45" s="5">
+      <c r="C45" s="4">
         <v>43806</v>
       </c>
-      <c r="D45" s="10"/>
+      <c r="D45" s="6"/>
     </row>
     <row r="46" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C46" s="5">
+      <c r="C46" s="4">
         <v>43807</v>
       </c>
-      <c r="D46" s="10"/>
+      <c r="D46" s="6"/>
     </row>
     <row r="47" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C47" s="5">
+      <c r="C47" s="4">
         <v>43808</v>
       </c>
-      <c r="D47" s="10"/>
+      <c r="D47" s="6"/>
     </row>
     <row r="48" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C48" s="5">
+      <c r="C48" s="4">
         <v>43809</v>
       </c>
-      <c r="D48" s="10"/>
+      <c r="D48" s="6"/>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C49" s="5">
+      <c r="C49" s="4">
         <v>43810</v>
       </c>
-      <c r="D49" s="10"/>
+      <c r="D49" s="6"/>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C50" s="5">
+      <c r="C50" s="4">
         <v>43811</v>
       </c>
-      <c r="D50" s="9"/>
+      <c r="D50" s="5"/>
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C51" s="5">
+      <c r="C51" s="4">
         <v>43812</v>
       </c>
-      <c r="D51" s="10"/>
+      <c r="D51" s="6"/>
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C52" s="5">
+      <c r="C52" s="4">
         <v>43813</v>
       </c>
-      <c r="D52" s="10"/>
+      <c r="D52" s="6"/>
     </row>
     <row r="53" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C53" s="5">
+      <c r="C53" s="4">
         <v>43814</v>
       </c>
-      <c r="D53" s="10"/>
+      <c r="D53" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="26">
+    <mergeCell ref="P22:W22"/>
+    <mergeCell ref="P23:W23"/>
+    <mergeCell ref="P24:W24"/>
+    <mergeCell ref="P25:W25"/>
+    <mergeCell ref="P26:W26"/>
+    <mergeCell ref="P17:W17"/>
+    <mergeCell ref="P18:W18"/>
+    <mergeCell ref="P19:W19"/>
+    <mergeCell ref="P20:W20"/>
+    <mergeCell ref="P21:W21"/>
+    <mergeCell ref="P12:W12"/>
+    <mergeCell ref="P13:W13"/>
+    <mergeCell ref="P14:W14"/>
+    <mergeCell ref="P15:W15"/>
+    <mergeCell ref="P16:W16"/>
+    <mergeCell ref="P7:W7"/>
+    <mergeCell ref="P8:W8"/>
+    <mergeCell ref="P9:W9"/>
+    <mergeCell ref="P10:W10"/>
+    <mergeCell ref="P11:W11"/>
     <mergeCell ref="C2:L3"/>
     <mergeCell ref="D6:N6"/>
+    <mergeCell ref="P2:W3"/>
+    <mergeCell ref="P4:W4"/>
+    <mergeCell ref="P5:W5"/>
+    <mergeCell ref="P6:W6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>